<commit_message>
Weeks 11 & 12 Updates
</commit_message>
<xml_diff>
--- a/Wins Fantasy League.xlsx
+++ b/Wins Fantasy League.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="26360" windowHeight="15980" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="25920" windowHeight="15980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -236,13 +236,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -296,7 +289,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="92">
+  <cellStyleXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -367,6 +360,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -421,12 +418,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="92">
+  <cellStyles count="96">
     <cellStyle name="Bad" xfId="69" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -473,6 +470,8 @@
     <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -518,269 +517,11 @@
     <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1191,7 +932,7 @@
   <dimension ref="A1:X33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1274,16 +1015,16 @@
         <v>23</v>
       </c>
       <c r="B2" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
       </c>
       <c r="D2" s="2">
-        <v>277</v>
+        <v>354</v>
       </c>
       <c r="E2" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" s="2" t="str">
         <f t="shared" ref="G2:K4" si="0">A2</f>
@@ -1291,7 +1032,7 @@
       </c>
       <c r="H2" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I2" s="2">
         <f t="shared" si="0"/>
@@ -1299,11 +1040,11 @@
       </c>
       <c r="J2" s="2">
         <f t="shared" si="0"/>
-        <v>277</v>
+        <v>354</v>
       </c>
       <c r="K2" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="str">
@@ -1312,15 +1053,15 @@
       </c>
       <c r="N2" s="2">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O2" s="2">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P2" s="2">
         <f t="shared" si="1"/>
-        <v>290</v>
+        <v>333</v>
       </c>
       <c r="Q2" s="2">
         <f t="shared" si="1"/>
@@ -1332,13 +1073,13 @@
         <v>24</v>
       </c>
       <c r="B3" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2">
         <v>6</v>
       </c>
       <c r="D3" s="2">
-        <v>194</v>
+        <v>236</v>
       </c>
       <c r="E3" s="2">
         <v>3</v>
@@ -1349,7 +1090,7 @@
       </c>
       <c r="H3" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" si="0"/>
@@ -1357,7 +1098,7 @@
       </c>
       <c r="J3" s="2">
         <f t="shared" si="0"/>
-        <v>194</v>
+        <v>236</v>
       </c>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
@@ -1370,7 +1111,7 @@
       </c>
       <c r="N3" s="2">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O3" s="2">
         <f t="shared" si="1"/>
@@ -1378,11 +1119,11 @@
       </c>
       <c r="P3" s="2">
         <f t="shared" si="1"/>
-        <v>261</v>
+        <v>288</v>
       </c>
       <c r="Q3" s="2">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S3" s="10" t="s">
         <v>47</v>
@@ -1398,16 +1139,16 @@
         <v>10</v>
       </c>
       <c r="B4" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="E4" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1415,19 +1156,19 @@
       </c>
       <c r="H4" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="0"/>
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="str">
@@ -1440,11 +1181,11 @@
       </c>
       <c r="O4" s="2">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P4" s="2">
         <f t="shared" si="1"/>
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="Q4" s="2">
         <f t="shared" si="1"/>
@@ -1474,13 +1215,13 @@
         <v>11</v>
       </c>
       <c r="B5" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="2">
-        <v>290</v>
+        <v>333</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
@@ -1490,19 +1231,19 @@
       </c>
       <c r="H5" s="3">
         <f>SUM(H2:H4)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I5" s="3">
         <f>SUM(I2:I4)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J5" s="3">
         <f>SUM(J2:J4)</f>
-        <v>680</v>
+        <v>832</v>
       </c>
       <c r="K5" s="3">
         <f>SUM(K2:K4)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="3" t="s">
@@ -1510,40 +1251,40 @@
       </c>
       <c r="N5" s="3">
         <f t="shared" ref="N5:O5" si="2">SUM(N2:N4)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O5" s="3">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="P5" s="3">
         <f>SUM(P2:P4)</f>
-        <v>709</v>
+        <v>782</v>
       </c>
       <c r="Q5" s="3">
         <f>SUM(Q2:Q4)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S5" s="6">
         <v>1</v>
       </c>
       <c r="T5" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U5" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="V5" s="2">
-        <f>$N$17</f>
-        <v>20</v>
+        <f>$H$29</f>
+        <v>22</v>
       </c>
       <c r="W5" s="2">
-        <f>$P$17</f>
-        <v>722</v>
+        <f>$J$29</f>
+        <v>891</v>
       </c>
       <c r="X5" s="2">
-        <f>$Q$17</f>
-        <v>7</v>
+        <f>$K$29</f>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="16" thickTop="1">
@@ -1551,16 +1292,16 @@
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2">
         <v>4</v>
       </c>
       <c r="D6" s="2">
-        <v>261</v>
+        <v>288</v>
       </c>
       <c r="E6" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -1577,21 +1318,21 @@
         <v>2</v>
       </c>
       <c r="T6" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="V6" s="2">
-        <f>$H$29</f>
-        <v>18</v>
+        <f>$N$17</f>
+        <v>22</v>
       </c>
       <c r="W6" s="2">
-        <f>$J$29</f>
-        <v>748</v>
+        <f>$P$17</f>
+        <v>834</v>
       </c>
       <c r="X6" s="2">
-        <f>$K$29</f>
+        <f>$Q$17</f>
         <v>8</v>
       </c>
     </row>
@@ -1603,10 +1344,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
@@ -1646,22 +1387,22 @@
         <v>3</v>
       </c>
       <c r="T7" s="6">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="V7" s="2">
-        <f>$H$23</f>
-        <v>16</v>
+        <f>$H$5</f>
+        <v>20</v>
       </c>
       <c r="W7" s="2">
-        <f>$J$23</f>
-        <v>637</v>
+        <f>$J$5</f>
+        <v>832</v>
       </c>
       <c r="X7" s="2">
-        <f>$K$23</f>
-        <v>5</v>
+        <f>$K$5</f>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -1669,16 +1410,16 @@
         <v>31</v>
       </c>
       <c r="B8" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
         <v>4</v>
       </c>
       <c r="D8" s="2">
-        <v>195</v>
+        <v>228</v>
       </c>
       <c r="E8" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G8" s="2" t="str">
         <f t="shared" ref="G8:K10" si="3">A8</f>
@@ -1686,7 +1427,7 @@
       </c>
       <c r="H8" s="2">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="3"/>
@@ -1694,11 +1435,11 @@
       </c>
       <c r="J8" s="2">
         <f t="shared" si="3"/>
-        <v>195</v>
+        <v>228</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2" t="str">
@@ -1711,11 +1452,11 @@
       </c>
       <c r="O8" s="2">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P8" s="2">
         <f t="shared" si="4"/>
-        <v>251</v>
+        <v>288</v>
       </c>
       <c r="Q8" s="2">
         <f t="shared" si="4"/>
@@ -1725,38 +1466,38 @@
         <v>4</v>
       </c>
       <c r="T8" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U8" s="6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="V8" s="2">
-        <f>$H$5</f>
-        <v>15</v>
+        <f>$H$23</f>
+        <v>18</v>
       </c>
       <c r="W8" s="2">
-        <f>$J$5</f>
-        <v>680</v>
+        <f>$J$23</f>
+        <v>696</v>
       </c>
       <c r="X8" s="2">
-        <f>$K$5</f>
-        <v>7</v>
+        <f>$K$23</f>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:24">
-      <c r="A9" t="s">
+      <c r="A9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="2">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2">
-        <v>195</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="B9" s="13">
+        <v>3</v>
+      </c>
+      <c r="C9" s="13">
+        <v>8</v>
+      </c>
+      <c r="D9" s="13">
+        <v>233</v>
+      </c>
+      <c r="E9" s="13">
         <v>1</v>
       </c>
       <c r="G9" s="2" t="str">
@@ -1769,11 +1510,11 @@
       </c>
       <c r="I9" s="2">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="3"/>
-        <v>195</v>
+        <v>233</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" si="3"/>
@@ -1786,7 +1527,7 @@
       </c>
       <c r="N9" s="2">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O9" s="2">
         <f t="shared" si="4"/>
@@ -1794,7 +1535,7 @@
       </c>
       <c r="P9" s="2">
         <f t="shared" si="4"/>
-        <v>205</v>
+        <v>245</v>
       </c>
       <c r="Q9" s="2">
         <f t="shared" si="4"/>
@@ -1804,38 +1545,38 @@
         <v>5</v>
       </c>
       <c r="T9" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="U9" s="6" t="s">
         <v>44</v>
       </c>
       <c r="V9" s="2">
         <f>$N$29</f>
-        <v>14.5</v>
+        <v>17.5</v>
       </c>
       <c r="W9" s="2">
         <f>$P$29</f>
-        <v>611</v>
+        <v>724</v>
       </c>
       <c r="X9" s="2">
         <f>$Q$29</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" t="s">
+      <c r="A10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>9</v>
-      </c>
-      <c r="D10" s="2">
-        <v>146</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" s="13">
+        <v>10</v>
+      </c>
+      <c r="D10" s="13">
+        <v>176</v>
+      </c>
+      <c r="E10" s="13">
         <v>0</v>
       </c>
       <c r="G10" s="2" t="str">
@@ -1844,15 +1585,15 @@
       </c>
       <c r="H10" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="3"/>
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" si="3"/>
@@ -1865,36 +1606,36 @@
       </c>
       <c r="N10" s="2">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O10" s="2">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P10" s="2">
         <f t="shared" si="4"/>
-        <v>219</v>
+        <v>262</v>
       </c>
       <c r="Q10" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S10" s="6">
         <v>6</v>
       </c>
       <c r="T10" s="6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="U10" s="9" t="s">
         <v>37</v>
       </c>
       <c r="V10" s="2">
         <f>$H$17</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="W10" s="2">
         <f>$J$17</f>
-        <v>657</v>
+        <v>809</v>
       </c>
       <c r="X10" s="2">
         <f>$K$17</f>
@@ -1902,19 +1643,19 @@
       </c>
     </row>
     <row r="11" spans="1:24" ht="16" thickBot="1">
-      <c r="A11" t="s">
+      <c r="A11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="2">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2">
-        <v>251</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="B11" s="13">
+        <v>4</v>
+      </c>
+      <c r="C11" s="13">
+        <v>7</v>
+      </c>
+      <c r="D11" s="13">
+        <v>288</v>
+      </c>
+      <c r="E11" s="13">
         <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -1922,19 +1663,19 @@
       </c>
       <c r="H11" s="3">
         <f>SUM(H8:H10)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I11" s="3">
         <f t="shared" ref="I11" si="5">SUM(I8:I10)</f>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="J11" s="3">
         <f>SUM(J8:J10)</f>
-        <v>536</v>
+        <v>637</v>
       </c>
       <c r="K11" s="3">
         <f>SUM(K8:K10)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="3" t="s">
@@ -1942,39 +1683,39 @@
       </c>
       <c r="N11" s="3">
         <f>SUM(N8:N10)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O11" s="3">
         <f>SUM(O8:O10)</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="P11" s="3">
         <f>SUM(P8:P10)</f>
-        <v>675</v>
+        <v>795</v>
       </c>
       <c r="Q11" s="3">
         <f>SUM(Q8:Q10)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S11" s="6">
         <v>7</v>
       </c>
       <c r="T11" s="6">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="U11" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="V11" s="2">
-        <f>$N$5</f>
-        <v>13</v>
+        <f>$N$11</f>
+        <v>15</v>
       </c>
       <c r="W11" s="2">
-        <f>$P$5</f>
-        <v>709</v>
+        <f>$P$11</f>
+        <v>795</v>
       </c>
       <c r="X11" s="2">
-        <f>$Q$5</f>
+        <f>$Q$11</f>
         <v>5</v>
       </c>
     </row>
@@ -1983,13 +1724,13 @@
         <v>16</v>
       </c>
       <c r="B12" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2">
         <v>4</v>
       </c>
       <c r="D12" s="2">
-        <v>205</v>
+        <v>245</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
@@ -2009,21 +1750,21 @@
         <v>8</v>
       </c>
       <c r="T12" s="6">
-        <v>8</v>
-      </c>
-      <c r="U12" s="9" t="s">
-        <v>43</v>
+        <v>6</v>
+      </c>
+      <c r="U12" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="V12" s="2">
-        <f>$N$23</f>
-        <v>12.5</v>
+        <f>$N$5</f>
+        <v>15</v>
       </c>
       <c r="W12" s="2">
-        <f>$P$23</f>
-        <v>557</v>
+        <f>$P$5</f>
+        <v>782</v>
       </c>
       <c r="X12" s="2">
-        <f>$Q$23</f>
+        <f>$Q$5</f>
         <v>6</v>
       </c>
     </row>
@@ -2032,16 +1773,16 @@
         <v>30</v>
       </c>
       <c r="B13" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" s="2">
-        <v>219</v>
+        <v>262</v>
       </c>
       <c r="E13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>37</v>
@@ -2080,36 +1821,36 @@
       <c r="T13" s="6">
         <v>9</v>
       </c>
-      <c r="U13" s="6" t="s">
-        <v>41</v>
+      <c r="U13" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="V13" s="2">
-        <f>$N$11</f>
-        <v>12</v>
+        <f>$N$23</f>
+        <v>13.5</v>
       </c>
       <c r="W13" s="2">
-        <f>$P$11</f>
-        <v>675</v>
+        <f>$P$23</f>
+        <v>655</v>
       </c>
       <c r="X13" s="2">
-        <f>$Q$11</f>
-        <v>4</v>
+        <f>$Q$23</f>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="12" t="s">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="13">
-        <v>7</v>
-      </c>
-      <c r="C14" s="13">
-        <v>2</v>
-      </c>
-      <c r="D14" s="13">
-        <v>286</v>
-      </c>
-      <c r="E14" s="13">
+      <c r="B14" s="2">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2">
+        <v>332</v>
+      </c>
+      <c r="E14" s="2">
         <v>2</v>
       </c>
       <c r="G14" s="2" t="str">
@@ -2118,15 +1859,15 @@
       </c>
       <c r="H14" s="2">
         <f t="shared" si="6"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="6"/>
-        <v>286</v>
+        <v>332</v>
       </c>
       <c r="K14" s="2">
         <f t="shared" si="6"/>
@@ -2139,15 +1880,15 @@
       </c>
       <c r="N14" s="2">
         <f t="shared" si="7"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O14" s="2">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P14" s="2">
         <f t="shared" si="7"/>
-        <v>279</v>
+        <v>342</v>
       </c>
       <c r="Q14" s="2">
         <f t="shared" si="7"/>
@@ -2164,15 +1905,15 @@
       </c>
       <c r="V14" s="2">
         <f>$H$11</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="W14" s="2">
         <f>$J$11</f>
-        <v>536</v>
+        <v>637</v>
       </c>
       <c r="X14" s="2">
         <f>$K$11</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:24">
@@ -2180,13 +1921,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="2">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2">
         <v>5</v>
       </c>
-      <c r="C15" s="2">
-        <v>4</v>
-      </c>
       <c r="D15" s="2">
-        <v>227</v>
+        <v>285</v>
       </c>
       <c r="E15" s="2">
         <v>3</v>
@@ -2197,15 +1938,15 @@
       </c>
       <c r="H15" s="2">
         <f>B15</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I15" s="2">
         <f>C15</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J15" s="2">
         <f>D15</f>
-        <v>227</v>
+        <v>285</v>
       </c>
       <c r="K15" s="2">
         <f>E15</f>
@@ -2218,7 +1959,7 @@
       </c>
       <c r="N15" s="2">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O15" s="2">
         <f t="shared" si="7"/>
@@ -2226,11 +1967,11 @@
       </c>
       <c r="P15" s="2">
         <f t="shared" si="7"/>
-        <v>261</v>
+        <v>295</v>
       </c>
       <c r="Q15" s="2">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:24">
@@ -2241,10 +1982,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D16" s="2">
-        <v>144</v>
+        <v>192</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
@@ -2259,11 +2000,11 @@
       </c>
       <c r="I16" s="2">
         <f t="shared" si="6"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="6"/>
-        <v>144</v>
+        <v>192</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="6"/>
@@ -2280,11 +2021,11 @@
       </c>
       <c r="O16" s="2">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P16" s="2">
         <f t="shared" si="7"/>
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="Q16" s="2">
         <f t="shared" si="7"/>
@@ -2296,13 +2037,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C17" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" s="2">
-        <v>279</v>
+        <v>342</v>
       </c>
       <c r="E17" s="2">
         <v>2</v>
@@ -2312,15 +2053,15 @@
       </c>
       <c r="H17" s="3">
         <f>SUM(H14:H16)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" ref="I17" si="8">SUM(I14:I16)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="J17" s="3">
         <f>SUM(J14:J16)</f>
-        <v>657</v>
+        <v>809</v>
       </c>
       <c r="K17" s="3">
         <f>SUM(K14:K16)</f>
@@ -2332,36 +2073,36 @@
       </c>
       <c r="N17" s="3">
         <f>SUM(N14:N16)</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O17" s="3">
         <f>SUM(O14:O16)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="P17" s="3">
         <f>SUM(P14:P16)</f>
-        <v>722</v>
+        <v>834</v>
       </c>
       <c r="Q17" s="3">
         <f>SUM(Q14:Q16)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="16" thickTop="1">
-      <c r="A18" t="s">
+      <c r="A18" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="2">
-        <v>6</v>
-      </c>
-      <c r="C18" s="2">
-        <v>4</v>
-      </c>
-      <c r="D18" s="2">
-        <v>261</v>
-      </c>
-      <c r="E18" s="2">
-        <v>2</v>
+      <c r="B18" s="13">
+        <v>7</v>
+      </c>
+      <c r="C18" s="13">
+        <v>4</v>
+      </c>
+      <c r="D18" s="13">
+        <v>295</v>
+      </c>
+      <c r="E18" s="13">
+        <v>3</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -2383,10 +2124,10 @@
         <v>7</v>
       </c>
       <c r="C19" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D19" s="2">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="E19" s="2">
         <v>3</v>
@@ -2428,13 +2169,13 @@
         <v>32</v>
       </c>
       <c r="B20" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C20" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D20" s="2">
-        <v>240</v>
+        <v>279</v>
       </c>
       <c r="E20" s="2">
         <v>2</v>
@@ -2445,15 +2186,15 @@
       </c>
       <c r="H20" s="2">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" si="9"/>
-        <v>240</v>
+        <v>279</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" si="9"/>
@@ -2470,11 +2211,11 @@
       </c>
       <c r="O20" s="2">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P20" s="2">
         <f t="shared" si="10"/>
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" si="10"/>
@@ -2486,13 +2227,13 @@
         <v>34</v>
       </c>
       <c r="B21" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C21" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="2">
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="E21" s="2">
         <v>3</v>
@@ -2503,15 +2244,15 @@
       </c>
       <c r="H21" s="2">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I21" s="2">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" si="9"/>
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="K21" s="2">
         <f t="shared" si="9"/>
@@ -2528,11 +2269,11 @@
       </c>
       <c r="O21" s="2">
         <f t="shared" si="10"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P21" s="2">
         <f t="shared" si="10"/>
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="Q21" s="2">
         <f t="shared" si="10"/>
@@ -2540,19 +2281,19 @@
       </c>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" t="s">
+      <c r="A22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="2">
-        <v>2</v>
-      </c>
-      <c r="C22" s="2">
-        <v>8</v>
-      </c>
-      <c r="D22" s="2">
-        <v>174</v>
-      </c>
-      <c r="E22" s="2">
+      <c r="B22" s="13">
+        <v>2</v>
+      </c>
+      <c r="C22" s="13">
+        <v>9</v>
+      </c>
+      <c r="D22" s="13">
+        <v>177</v>
+      </c>
+      <c r="E22" s="13">
         <v>0</v>
       </c>
       <c r="G22" s="2" t="str">
@@ -2565,11 +2306,11 @@
       </c>
       <c r="I22" s="2">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J22" s="2">
         <f t="shared" si="9"/>
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="K22" s="2">
         <f t="shared" si="9"/>
@@ -2582,15 +2323,15 @@
       </c>
       <c r="N22" s="2">
         <f>B25</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O22" s="2">
         <f>C25</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P22" s="2">
         <f>D25</f>
-        <v>191</v>
+        <v>238</v>
       </c>
       <c r="Q22" s="2">
         <f>E25</f>
@@ -2605,10 +2346,10 @@
         <v>4</v>
       </c>
       <c r="C23" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D23" s="2">
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="E23" s="2">
         <v>2</v>
@@ -2618,15 +2359,15 @@
       </c>
       <c r="H23" s="3">
         <f>SUM(H20:H22)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I23" s="3">
         <f t="shared" ref="I23" si="11">SUM(I20:I22)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J23" s="3">
         <f>SUM(J20:J22)</f>
-        <v>637</v>
+        <v>696</v>
       </c>
       <c r="K23" s="3">
         <f>SUM(K20:K22)</f>
@@ -2638,15 +2379,15 @@
       </c>
       <c r="N23" s="3">
         <f>SUM(N20:N22)</f>
-        <v>12.5</v>
+        <v>13.5</v>
       </c>
       <c r="O23" s="3">
         <f>SUM(O20:O22)</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="P23" s="3">
         <f>SUM(P20:P22)</f>
-        <v>557</v>
+        <v>655</v>
       </c>
       <c r="Q23" s="3">
         <f>SUM(Q20:Q22)</f>
@@ -2661,10 +2402,10 @@
         <v>3.5</v>
       </c>
       <c r="C24" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D24" s="2">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="E24" s="2">
         <v>1</v>
@@ -2682,19 +2423,19 @@
       <c r="Q24" s="2"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="2">
+      <c r="A25" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="13">
+        <v>6</v>
+      </c>
+      <c r="C25" s="13">
         <v>5</v>
       </c>
-      <c r="C25" s="2">
-        <v>4</v>
-      </c>
-      <c r="D25" s="2">
-        <v>191</v>
-      </c>
-      <c r="E25" s="2">
+      <c r="D25" s="13">
+        <v>238</v>
+      </c>
+      <c r="E25" s="13">
         <v>3</v>
       </c>
       <c r="G25" s="4" t="s">
@@ -2734,16 +2475,16 @@
         <v>0</v>
       </c>
       <c r="B26" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C26" s="2">
         <v>2</v>
       </c>
       <c r="D26" s="2">
-        <v>281</v>
+        <v>357</v>
       </c>
       <c r="E26" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G26" s="2" t="str">
         <f t="shared" ref="G26:K28" si="12">A26</f>
@@ -2751,7 +2492,7 @@
       </c>
       <c r="H26" s="2">
         <f t="shared" si="12"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I26" s="2">
         <f t="shared" si="12"/>
@@ -2759,11 +2500,11 @@
       </c>
       <c r="J26" s="2">
         <f t="shared" si="12"/>
-        <v>281</v>
+        <v>357</v>
       </c>
       <c r="K26" s="2">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="2" t="str">
@@ -2772,15 +2513,15 @@
       </c>
       <c r="N26" s="2">
         <f t="shared" si="13"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O26" s="2">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P26" s="2">
         <f t="shared" si="13"/>
-        <v>217</v>
+        <v>261</v>
       </c>
       <c r="Q26" s="2">
         <f t="shared" si="13"/>
@@ -2788,20 +2529,20 @@
       </c>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" t="s">
+      <c r="A27" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="2">
-        <v>7</v>
-      </c>
-      <c r="C27" s="2">
-        <v>3</v>
-      </c>
-      <c r="D27" s="2">
-        <v>261</v>
-      </c>
-      <c r="E27" s="2">
-        <v>4</v>
+      <c r="B27" s="13">
+        <v>8</v>
+      </c>
+      <c r="C27" s="13">
+        <v>3</v>
+      </c>
+      <c r="D27" s="13">
+        <v>292</v>
+      </c>
+      <c r="E27" s="13">
+        <v>5</v>
       </c>
       <c r="G27" s="2" t="str">
         <f t="shared" si="12"/>
@@ -2809,7 +2550,7 @@
       </c>
       <c r="H27" s="2">
         <f t="shared" si="12"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I27" s="2">
         <f t="shared" si="12"/>
@@ -2817,11 +2558,11 @@
       </c>
       <c r="J27" s="2">
         <f t="shared" si="12"/>
-        <v>261</v>
+        <v>292</v>
       </c>
       <c r="K27" s="2">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2" t="str">
@@ -2830,7 +2571,7 @@
       </c>
       <c r="N27" s="2">
         <f t="shared" si="13"/>
-        <v>5.5</v>
+        <v>7.5</v>
       </c>
       <c r="O27" s="2">
         <f t="shared" si="13"/>
@@ -2838,11 +2579,11 @@
       </c>
       <c r="P27" s="2">
         <f t="shared" si="13"/>
-        <v>197</v>
+        <v>246</v>
       </c>
       <c r="Q27" s="2">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -2850,16 +2591,16 @@
         <v>14</v>
       </c>
       <c r="B28" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C28" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D28" s="2">
-        <v>206</v>
+        <v>242</v>
       </c>
       <c r="E28" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G28" s="2" t="str">
         <f t="shared" si="12"/>
@@ -2867,19 +2608,19 @@
       </c>
       <c r="H28" s="2">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I28" s="2">
         <f t="shared" si="12"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J28" s="2">
         <f t="shared" si="12"/>
-        <v>206</v>
+        <v>242</v>
       </c>
       <c r="K28" s="2">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2" t="str">
@@ -2892,11 +2633,11 @@
       </c>
       <c r="O28" s="2">
         <f t="shared" si="13"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="P28" s="2">
         <f t="shared" si="13"/>
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="Q28" s="2">
         <f t="shared" si="13"/>
@@ -2908,13 +2649,13 @@
         <v>17</v>
       </c>
       <c r="B29" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C29" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D29" s="2">
-        <v>217</v>
+        <v>261</v>
       </c>
       <c r="E29" s="2">
         <v>3</v>
@@ -2924,19 +2665,19 @@
       </c>
       <c r="H29" s="3">
         <f>SUM(H26:H28)</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I29" s="3">
         <f t="shared" ref="I29" si="14">SUM(I26:I28)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J29" s="3">
         <f>SUM(J26:J28)</f>
-        <v>748</v>
+        <v>891</v>
       </c>
       <c r="K29" s="3">
         <f>SUM(K26:K28)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="3" t="s">
@@ -2944,19 +2685,19 @@
       </c>
       <c r="N29" s="3">
         <f>SUM(N26:N28)</f>
-        <v>14.5</v>
+        <v>17.5</v>
       </c>
       <c r="O29" s="3">
         <f>SUM(O26:O28)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="P29" s="3">
         <f>SUM(P26:P28)</f>
-        <v>611</v>
+        <v>724</v>
       </c>
       <c r="Q29" s="3">
         <f>SUM(Q26:Q28)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="16" thickTop="1">
@@ -2964,16 +2705,16 @@
         <v>7</v>
       </c>
       <c r="B30" s="2">
-        <v>5.5</v>
+        <v>7.5</v>
       </c>
       <c r="C30" s="2">
         <v>3</v>
       </c>
       <c r="D30" s="2">
-        <v>197</v>
+        <v>246</v>
       </c>
       <c r="E30" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -2984,10 +2725,10 @@
         <v>3</v>
       </c>
       <c r="C31" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D31" s="2">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="E31" s="2">
         <v>1</v>
@@ -2998,13 +2739,13 @@
         <v>33</v>
       </c>
       <c r="B32" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C32" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D32" s="8">
-        <v>163</v>
+        <v>209</v>
       </c>
       <c r="E32" s="8">
         <v>2</v>
@@ -3016,7 +2757,7 @@
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
       <c r="K32" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3024,16 +2765,16 @@
         <v>29</v>
       </c>
       <c r="B33" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33" s="8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D33" s="8">
-        <v>167</v>
+        <v>207</v>
       </c>
       <c r="E33" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3047,30 +2788,30 @@
     <mergeCell ref="G32:J32"/>
   </mergeCells>
   <conditionalFormatting sqref="D32:D33">
-    <cfRule type="containsText" dxfId="33" priority="43" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="7" priority="55" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",D32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="44" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="6" priority="56" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",D32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S5:S14">
-    <cfRule type="cellIs" dxfId="31" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="37" operator="greaterThan">
       <formula>T5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="38" operator="equal">
       <formula>T5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="39" operator="lessThan">
       <formula>T5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="51" operator="equal">
       <formula>T5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="52" operator="lessThan">
       <formula>T5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="53" operator="greaterThan">
       <formula>T5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>